<commit_message>
Changes from sprint 1 review
</commit_message>
<xml_diff>
--- a/assignment8/src/Backlog/Product Backlog.xlsx
+++ b/assignment8/src/Backlog/Product Backlog.xlsx
@@ -9,8 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -41,13 +40,13 @@
     <t>Whenever I enter an event (5K, 5-mile, 10K, half-marathon), and pace, the app tells me how much time it would take to run that distance.</t>
   </si>
   <si>
-    <t>GUI interface</t>
-  </si>
-  <si>
     <t>Product Backlog</t>
   </si>
   <si>
-    <t>AE</t>
+    <t>User stories only</t>
+  </si>
+  <si>
+    <t>functional</t>
   </si>
 </sst>
 </file>
@@ -501,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,12 +514,12 @@
     <col min="5" max="5" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C1" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>1</v>
@@ -535,7 +534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -544,7 +543,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9">
         <v>1</v>
@@ -555,7 +554,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9">
         <v>2</v>
@@ -566,7 +565,7 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9">
         <v>3</v>
@@ -577,22 +576,19 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="9">
-        <v>3</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9">
         <v>5</v>
@@ -600,36 +596,39 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>

</xml_diff>

<commit_message>
Added client answers to product backlog.
</commit_message>
<xml_diff>
--- a/assignment8/src/Backlog/Product Backlog.xlsx
+++ b/assignment8/src/Backlog/Product Backlog.xlsx
@@ -31,15 +31,6 @@
     <t>By</t>
   </si>
   <si>
-    <t>Whenever I enter a time and event (5K, 5-mile, 10K, half-marathon), the app tells me what my pace should be (during prep) or was (if completed).</t>
-  </si>
-  <si>
-    <t>Whenever I enter a time and pace, the app tells me how far I could run.</t>
-  </si>
-  <si>
-    <t>Whenever I enter an event (5K, 5-mile, 10K, half-marathon), and pace, the app tells me how much time it would take to run that distance.</t>
-  </si>
-  <si>
     <t>Product Backlog</t>
   </si>
   <si>
@@ -47,6 +38,17 @@
   </si>
   <si>
     <t>functional</t>
+  </si>
+  <si>
+    <t>Whenever I enter a time and pace, the app tells me how far I could run. In miles.</t>
+  </si>
+  <si>
+    <t>Whenever I enter a time and event (5K, 5-mile, 10K, half-marathon), the app tells me what my pace should be (during prep) or was (if completed). Pace must be displayed as minutes, seconds, and tenths of seconds per mile, e.g., 7:03.6
+Pace must have an upper limit of 20 min/mile. Only one decimal digit.</t>
+  </si>
+  <si>
+    <t>Whenever I enter an event (5K, 5-mile, 10K, half-marathon), and pace, the app tells me how much time it would take to run that distance.  Time must be displayed as hours, minutes, seconds, and tenths of seconds, e.g., 1:43:54.7
+Time has an upper limit of 4 hours.  Only one decimal digit.  Only whole values for hours are allowed.</t>
   </si>
 </sst>
 </file>
@@ -503,7 +505,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +518,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C1" s="11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -543,13 +545,13 @@
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="126" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -560,18 +562,18 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9">
         <v>3</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -585,7 +587,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -597,7 +599,7 @@
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Product and Sprint 2 Backlogs formated to turn in.
</commit_message>
<xml_diff>
--- a/assignment8/src/Backlog/Product Backlog.xlsx
+++ b/assignment8/src/Backlog/Product Backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Very High</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t>Product Backlog</t>
-  </si>
-  <si>
-    <t>User stories only</t>
-  </si>
-  <si>
-    <t>functional</t>
   </si>
   <si>
     <t>Whenever I enter a time and pace, the app tells me how far I could run. In miles.</t>
@@ -49,6 +43,9 @@
   <si>
     <t>Whenever I enter an event (5K, 5-mile, 10K, half-marathon), and pace, the app tells me how much time it would take to run that distance.  Time must be displayed as hours, minutes, seconds, and tenths of seconds, e.g., 1:43:54.7
 Time has an upper limit of 4 hours.  Only one decimal digit.  Only whole values for hours are allowed.</t>
+  </si>
+  <si>
+    <t>Team 4</t>
   </si>
 </sst>
 </file>
@@ -502,26 +499,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="44" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>1</v>
@@ -536,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -545,98 +540,72 @@
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="9">
+        <v>24</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9">
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D5" s="9">
+        <v>24</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9">
         <v>3</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D6" s="9">
+        <v>24</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
-      <c r="B7" s="9">
-        <v>4</v>
-      </c>
+      <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="G7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
-      <c r="B8" s="9">
-        <v>5</v>
-      </c>
+      <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>